<commit_message>
combining b10brf and b10brm into b10br
</commit_message>
<xml_diff>
--- a/Final_Figures_and_Sheets_Superset/Kb_pc_values_CDR3.xlsx
+++ b/Final_Figures_and_Sheets_Superset/Kb_pc_values_CDR3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M112"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>0.004004076352098526</v>
+        <v>0</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2716,17 +2716,17 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × B10BRM|RTY</t>
+          <t>B10BR|RTY × BALBc|RTY</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
@@ -2743,7 +2743,7 @@
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>SNY</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
@@ -2752,22 +2752,22 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>SNY</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>SNY</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × BALBc|RTY</t>
+          <t>B10BR|SNY × BALBc|SNY</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -2789,31 +2789,31 @@
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>VGP</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>0.0005690102777481419</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>VGP</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>VGP</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>B10BRM|RTY × BALBc|RTY</t>
+          <t>B10BR|VGP × BALBc|VGP</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
@@ -2828,313 +2828,316 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>L3: within epitope
-across strain</t>
+          <t>L4: within strain
+across epitope</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
       <c r="E59" t="n">
-        <v>0.009223719254269153</v>
+        <v>0.001212469289429182</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>B10BRF|SNY × B10BRM|SNY</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr"/>
+          <t>B10BR|RTY × B10BR|SNY</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>RTY</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>SNY</t>
+        </is>
+      </c>
       <c r="M59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>L3: within epitope
-across strain</t>
+          <t>L4: within strain
+across epitope</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>0.0001587793926503604</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>B10BRF|SNY × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr"/>
-      <c r="L60" t="inlineStr"/>
+          <t>B10BR|RTY × B10BR|VGP</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>RTY</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>VGP</t>
+        </is>
+      </c>
       <c r="M60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>L3: within epitope
-across strain</t>
+          <t>L4: within strain
+across epitope</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>0.0001263573222030195</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>B10BRM|SNY × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr"/>
-      <c r="L61" t="inlineStr"/>
+          <t>B10BR|SNY × B10BR|VGP</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>SNY</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>VGP</t>
+        </is>
+      </c>
       <c r="M61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>L3: within epitope
-across strain</t>
+          <t>L4: within strain
+across epitope</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="E62" t="n">
-        <v>0.006873693834900731</v>
+        <v>0.004293738298314957</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>B10BRF|VGP × B10BRM|VGP</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr"/>
-      <c r="L62" t="inlineStr"/>
+          <t>BALBc|RTY × BALBc|SNY</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>RTY</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>SNY</t>
+        </is>
+      </c>
       <c r="M62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>L3: within epitope
-across strain</t>
+          <t>L4: within strain
+across epitope</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="E63" t="n">
-        <v>6.129253702069236e-05</v>
+        <v>0.002328050449620732</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>B10BRF|VGP × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr"/>
-      <c r="L63" t="inlineStr"/>
+          <t>BALBc|RTY × BALBc|VGP</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>RTY</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>VGP</t>
+        </is>
+      </c>
       <c r="M63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>L3: within epitope
-across strain</t>
+          <t>L4: within strain
+across epitope</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="E64" t="n">
-        <v>0.0008578841647137596</v>
+        <v>0.004387668199625277</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>B10BRM|VGP × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr"/>
-      <c r="L64" t="inlineStr"/>
+          <t>BALBc|SNY × BALBc|VGP</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>SNY</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>VGP</t>
+        </is>
+      </c>
       <c r="M64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
+      <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>0.002703835673862922</v>
+        <v>0.001212469289429182</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × B10BRF|SNY</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr"/>
-      <c r="J65" t="inlineStr"/>
+          <t>B10BR|RTY × B10BR|SNY</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
       <c r="K65" t="inlineStr">
         <is>
           <t>RTY</t>
@@ -3150,37 +3153,40 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
+      <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
-        <v>0.0007431260837255387</v>
+        <v>0.0001587793926503604</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × B10BRF|VGP</t>
-        </is>
-      </c>
-      <c r="I66" t="inlineStr"/>
-      <c r="J66" t="inlineStr"/>
+          <t>B10BR|RTY × B10BR|VGP</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
       <c r="K66" t="inlineStr">
         <is>
           <t>RTY</t>
@@ -3196,45 +3202,48 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
+      <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
         <v>0</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>B10BRF|SNY × B10BRF|VGP</t>
-        </is>
-      </c>
-      <c r="I67" t="inlineStr"/>
-      <c r="J67" t="inlineStr"/>
+          <t>B10BR|RTY × BALBc|RTY</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>RTY</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>RTY</t>
         </is>
       </c>
       <c r="M67" t="inlineStr"/>
@@ -3242,37 +3251,40 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>0.0008265489689747011</v>
+        <v>0</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>B10BRM|RTY × B10BRM|SNY</t>
-        </is>
-      </c>
-      <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr"/>
+          <t>B10BR|RTY × BALBc|SNY</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="K68" t="inlineStr">
         <is>
           <t>RTY</t>
@@ -3288,37 +3300,40 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
+      <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
-        <v>5.716637702368975e-06</v>
+        <v>0</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>B10BRM|RTY × B10BRM|VGP</t>
-        </is>
-      </c>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
+          <t>B10BR|RTY × BALBc|VGP</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="K69" t="inlineStr">
         <is>
           <t>RTY</t>
@@ -3334,37 +3349,40 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
+      <c r="D70" t="inlineStr"/>
       <c r="E70" t="n">
-        <v>0.0001448486551021841</v>
+        <v>0.0001263573222030195</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>B10BRM|SNY × B10BRM|VGP</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
+          <t>B10BR|SNY × B10BR|VGP</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
       <c r="K70" t="inlineStr">
         <is>
           <t>SNY</t>
@@ -3380,45 +3398,48 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
+      <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
-        <v>0.004293738298314957</v>
+        <v>0</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>BALBc</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>BALBc</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>BALBc|RTY × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr"/>
-      <c r="J71" t="inlineStr"/>
+          <t>B10BR|SNY × BALBc|RTY</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>SNY</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>RTY</t>
         </is>
       </c>
       <c r="M71" t="inlineStr"/>
@@ -3426,45 +3447,48 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
+      <c r="D72" t="inlineStr"/>
       <c r="E72" t="n">
-        <v>0.002328050449620732</v>
+        <v>0</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>BALBc</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>BALBc</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>BALBc|RTY × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I72" t="inlineStr"/>
-      <c r="J72" t="inlineStr"/>
+          <t>B10BR|SNY × BALBc|SNY</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>SNY</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>SNY</t>
         </is>
       </c>
       <c r="M72" t="inlineStr"/>
@@ -3472,37 +3496,40 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>L4: within strain
-across epitope</t>
+          <t>L5: all supersets</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
+      <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
-        <v>0.004387668199625277</v>
+        <v>0</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>BALBc</t>
+          <t>All</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>BALBc</t>
+          <t>All</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>BALBc|SNY × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr"/>
-      <c r="J73" t="inlineStr"/>
+          <t>B10BR|SNY × BALBc|VGP</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="K73" t="inlineStr">
         <is>
           <t>SNY</t>
@@ -3525,7 +3552,7 @@
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="n">
-        <v>0.002703835673862922</v>
+        <v>0</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -3539,27 +3566,27 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × B10BRF|SNY</t>
+          <t>B10BR|VGP × BALBc|RTY</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>VGP</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>SNY</t>
+          <t>RTY</t>
         </is>
       </c>
       <c r="M74" t="inlineStr"/>
@@ -3574,7 +3601,7 @@
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="n">
-        <v>0.0007431260837255387</v>
+        <v>0</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -3588,27 +3615,27 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × B10BRF|VGP</t>
+          <t>B10BR|VGP × BALBc|SNY</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>VGP</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>VGP</t>
+          <t>SNY</t>
         </is>
       </c>
       <c r="M75" t="inlineStr"/>
@@ -3623,7 +3650,7 @@
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
-        <v>0.004004076352098526</v>
+        <v>0.0005690102777481419</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -3637,27 +3664,27 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × B10BRM|RTY</t>
+          <t>B10BR|VGP × BALBc|VGP</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>B10BR</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>VGP</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>VGP</t>
         </is>
       </c>
       <c r="M76" t="inlineStr"/>
@@ -3672,7 +3699,7 @@
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="n">
-        <v>0.001043302607701571</v>
+        <v>0.004293738298314957</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -3686,17 +3713,17 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × B10BRM|SNY</t>
+          <t>BALBc|RTY × BALBc|SNY</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -3721,7 +3748,7 @@
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="n">
-        <v>5.872404397256412e-05</v>
+        <v>0.002328050449620732</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -3735,17 +3762,17 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × B10BRM|VGP</t>
+          <t>BALBc|RTY × BALBc|VGP</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>B10BRM</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -3770,7 +3797,7 @@
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>0.004387668199625277</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -3784,12 +3811,12 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>B10BRF|RTY × BALBc|RTY</t>
+          <t>BALBc|SNY × BALBc|VGP</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>B10BRF</t>
+          <t>BALBc</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
@@ -3799,12 +3826,12 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>SNY</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>RTY</t>
+          <t>VGP</t>
         </is>
       </c>
       <c r="M79" t="inlineStr"/>
@@ -3812,1579 +3839,109 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>L5: all supersets</t>
+          <t>L6: pre-immune</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>B10BR</t>
+        </is>
+      </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>2.421027674426409e-08</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>B10BR SLO</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>B10BRF|RTY × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr"/>
+          <t>B10BR</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>individual</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>L5: all supersets</t>
+          <t>L6: pre-immune</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>BALBc</t>
+        </is>
+      </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>1.949841837061067e-08</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>BALBc SLO</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>B10BRF|RTY × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr"/>
+          <t>BALBc</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>individual</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>L5: all supersets</t>
+          <t>L6: pre-immune</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>B10BR × BALBc</t>
+        </is>
+      </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>8.7710385535849e-10</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>B10BR × BALBc</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>B10BRF|SNY × B10BRF|VGP</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr"/>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="n">
-        <v>0.0002805549887778004</v>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>B10BRF|SNY × B10BRM|RTY</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr"/>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="n">
-        <v>0.009223719254269153</v>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>B10BRF|SNY × B10BRM|SNY</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="n">
-        <v>0.0002445291777188329</v>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>B10BRF|SNY × B10BRM|VGP</t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M85" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="n">
-        <v>0</v>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>B10BRF|SNY × BALBc|RTY</t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="n">
-        <v>0</v>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>B10BRF|SNY × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="n">
-        <v>0</v>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>B10BRF|SNY × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="n">
-        <v>3.014227152158187e-05</v>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>B10BRF|VGP × B10BRM|RTY</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="n">
-        <v>7.714620749243968e-06</v>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>B10BRF|VGP × B10BRM|SNY</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="n">
-        <v>0.006873693834900731</v>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>B10BRF|VGP × B10BRM|VGP</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr"/>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="n">
-        <v>0</v>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>B10BRF|VGP × BALBc|RTY</t>
-        </is>
-      </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="n">
-        <v>0</v>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>B10BRF|VGP × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr"/>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="n">
-        <v>6.129253702069236e-05</v>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>B10BRF|VGP × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>B10BRF</t>
-        </is>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr"/>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="n">
-        <v>0.0008265489689747011</v>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>B10BRM|RTY × B10BRM|SNY</t>
-        </is>
-      </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr"/>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="n">
-        <v>5.716637702368975e-06</v>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>B10BRM|RTY × B10BRM|VGP</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr"/>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="n">
-        <v>0</v>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>B10BRM|RTY × BALBc|RTY</t>
-        </is>
-      </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J97" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="M97" t="inlineStr"/>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="n">
-        <v>0</v>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>B10BRM|RTY × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M98" t="inlineStr"/>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="n">
-        <v>0</v>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>B10BRM|RTY × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J99" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr"/>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
-      <c r="E100" t="n">
-        <v>0.0001448486551021841</v>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>B10BRM|SNY × B10BRM|VGP</t>
-        </is>
-      </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr"/>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr"/>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="n">
-        <v>0</v>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>B10BRM|SNY × BALBc|RTY</t>
-        </is>
-      </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J101" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr"/>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr"/>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="n">
-        <v>0</v>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>B10BRM|SNY × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M102" t="inlineStr"/>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr"/>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="n">
-        <v>0</v>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>B10BRM|SNY × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J103" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M103" t="inlineStr"/>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr"/>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="n">
-        <v>0</v>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>B10BRM|VGP × BALBc|RTY</t>
-        </is>
-      </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr"/>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr"/>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="n">
-        <v>0</v>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>B10BRM|VGP × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J105" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L105" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M105" t="inlineStr"/>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="n">
-        <v>0.0008578841647137596</v>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>B10BRM|VGP × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>B10BRM</t>
-        </is>
-      </c>
-      <c r="J106" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="L106" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M106" t="inlineStr"/>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="n">
-        <v>0.004293738298314957</v>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>BALBc|RTY × BALBc|SNY</t>
-        </is>
-      </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="J107" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L107" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="M107" t="inlineStr"/>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr"/>
-      <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="n">
-        <v>0.002328050449620732</v>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>BALBc|RTY × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="J108" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K108" t="inlineStr">
-        <is>
-          <t>RTY</t>
-        </is>
-      </c>
-      <c r="L108" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M108" t="inlineStr"/>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>L5: all supersets</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr"/>
-      <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr"/>
-      <c r="E109" t="n">
-        <v>0.004387668199625277</v>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>BALBc|SNY × BALBc|VGP</t>
-        </is>
-      </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="J109" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>SNY</t>
-        </is>
-      </c>
-      <c r="L109" t="inlineStr">
-        <is>
-          <t>VGP</t>
-        </is>
-      </c>
-      <c r="M109" t="inlineStr"/>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>L6: pre-immune</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr"/>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>B10BR</t>
-        </is>
-      </c>
-      <c r="E110" t="n">
-        <v>2.421027674426409e-08</v>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>B10BR SLO</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>B10BR</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr"/>
-      <c r="I110" t="inlineStr"/>
-      <c r="J110" t="inlineStr"/>
-      <c r="K110" t="inlineStr"/>
-      <c r="L110" t="inlineStr"/>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>individual</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>L6: pre-immune</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr"/>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="E111" t="n">
-        <v>1.949841837061067e-08</v>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>BALBc SLO</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>BALBc</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr"/>
-      <c r="I111" t="inlineStr"/>
-      <c r="J111" t="inlineStr"/>
-      <c r="K111" t="inlineStr"/>
-      <c r="L111" t="inlineStr"/>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>individual</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>L6: pre-immune</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr"/>
-      <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>B10BR × BALBc</t>
-        </is>
-      </c>
-      <c r="E112" t="n">
-        <v>8.7710385535849e-10</v>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>B10BR × BALBc</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
           <t>Cross</t>
         </is>
       </c>
-      <c r="H112" t="inlineStr"/>
-      <c r="I112" t="inlineStr"/>
-      <c r="J112" t="inlineStr"/>
-      <c r="K112" t="inlineStr"/>
-      <c r="L112" t="inlineStr"/>
-      <c r="M112" t="inlineStr">
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr">
         <is>
           <t>cross</t>
         </is>

</xml_diff>